<commit_message>
as discussed in team call 16-4
</commit_message>
<xml_diff>
--- a/doc/planning/planning_gantt.xlsx
+++ b/doc/planning/planning_gantt.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruthv\PycharmProjects\infovis\doc\planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\python\infovis\doc\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58D0C4D-29B3-4EB7-B6E8-4CF3AAB3B50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23258" windowHeight="12458"/>
   </bookViews>
   <sheets>
     <sheet name="planning" sheetId="13" r:id="rId1"/>
@@ -18,12 +17,12 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">planning!$A$3:$IK$33</definedName>
+    <definedName name="helpRow">planning!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">planning!$A$1:$IK$33</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">planning!$1:$3</definedName>
-    <definedName name="helpRow">planning!#REF!</definedName>
     <definedName name="valuevx">42.314159</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -41,12 +40,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Jon</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="D3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -193,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="E3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -304,7 +303,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="F3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -330,7 +329,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="G3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -356,7 +355,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="H3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -382,7 +381,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="I3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -505,15 +504,9 @@
     <t>clinic: interim presentations</t>
   </si>
   <si>
-    <t>sprint 1: data processing / aggregation / filters</t>
-  </si>
-  <si>
     <t>sprint 1: bar charts, BAN, popups</t>
   </si>
   <si>
-    <t>sprint 1: map plot</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -536,12 +529,18 @@
   </si>
   <si>
     <t>online interim presentation</t>
+  </si>
+  <si>
+    <t>sprint 1: data processing / aggregation / filters / interactivity</t>
+  </si>
+  <si>
+    <t>sprint 1: map plot (framework selection, notebook impl)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd\ mmm\ yy"/>
     <numFmt numFmtId="165" formatCode="ddd\ dd/mm/yy"/>
@@ -1143,19 +1142,19 @@
     <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="25" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="Check Cell" xfId="26" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Explanatory Text" xfId="27" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Heading 1" xfId="28" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="Heading 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Heading 3" xfId="30" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="Heading 4" xfId="31" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="Input" xfId="32" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="Normal 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Note" xfId="34" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="Output" xfId="35" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Procent" xfId="36" builtinId="5"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Bad" xfId="25"/>
+    <cellStyle name="Check Cell" xfId="26"/>
+    <cellStyle name="Explanatory Text" xfId="27"/>
+    <cellStyle name="Heading 1" xfId="28"/>
+    <cellStyle name="Heading 2" xfId="29"/>
+    <cellStyle name="Heading 3" xfId="30"/>
+    <cellStyle name="Heading 4" xfId="31"/>
+    <cellStyle name="Input" xfId="32"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="33"/>
+    <cellStyle name="Note" xfId="34"/>
+    <cellStyle name="Output" xfId="35"/>
+    <cellStyle name="Percent" xfId="36" builtinId="5"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -1290,13 +1289,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>22860</xdr:rowOff>
+          <xdr:rowOff>23813</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>381000</xdr:colOff>
+          <xdr:colOff>139212</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
@@ -1659,7 +1658,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5">
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="1"/>
@@ -1667,23 +1666,23 @@
   <dimension ref="A1:IK33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22:F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.109375" customWidth="1"/>
+    <col min="1" max="1" width="30.53125" customWidth="1"/>
     <col min="2" max="2" width="5.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
-    <col min="5" max="5" width="6.109375" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1328125" customWidth="1"/>
+    <col min="4" max="4" width="10.46484375" customWidth="1"/>
+    <col min="5" max="5" width="6.1328125" customWidth="1"/>
+    <col min="6" max="6" width="9.1328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="1" customWidth="1"/>
-    <col min="8" max="245" width="0.44140625" customWidth="1"/>
+    <col min="8" max="245" width="0.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:245" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:245" ht="15" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -1695,7 +1694,7 @@
       </c>
       <c r="F1" s="19">
         <f ca="1">TODAY()</f>
-        <v>45392</v>
+        <v>45398</v>
       </c>
       <c r="G1" s="19">
         <v>45323</v>
@@ -1718,7 +1717,7 @@
       <c r="U1" s="17"/>
       <c r="V1" s="17"/>
     </row>
-    <row r="2" spans="1:245" s="1" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:245" s="1" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="20"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -2679,7 +2678,7 @@
         <v>45557</v>
       </c>
     </row>
-    <row r="3" spans="1:245" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:245" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="12" t="s">
         <v>8</v>
       </c>
@@ -3040,7 +3039,7 @@
       <c r="IJ3" s="33"/>
       <c r="IK3" s="34"/>
     </row>
-    <row r="4" spans="1:245" s="15" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:245" s="15" customFormat="1" ht="10.15" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>11</v>
       </c>
@@ -3061,7 +3060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:245" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:245" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
@@ -3082,7 +3081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:245" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:245" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
@@ -3103,7 +3102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:245" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:245" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>21</v>
       </c>
@@ -3125,7 +3124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:245" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:245" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
@@ -3146,7 +3145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:245" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:245" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
@@ -3167,7 +3166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:245" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:245" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>17</v>
       </c>
@@ -3189,7 +3188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:245" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:245" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -3211,7 +3210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:245" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:245" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>19</v>
       </c>
@@ -3232,7 +3231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:245" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:245" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>23</v>
       </c>
@@ -3253,7 +3252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:245" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:245" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>24</v>
       </c>
@@ -3274,7 +3273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:245" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:245" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>25</v>
       </c>
@@ -3292,12 +3291,12 @@
         <v>7</v>
       </c>
       <c r="F15" s="8">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:245" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:245" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>20</v>
@@ -3314,10 +3313,10 @@
         <v>7</v>
       </c>
       <c r="F16" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:112" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:112" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>26</v>
       </c>
@@ -3335,12 +3334,12 @@
         <v>1</v>
       </c>
       <c r="F17" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:112" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:112" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>15</v>
@@ -3359,7 +3358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:112" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:112" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>27</v>
       </c>
@@ -3383,7 +3382,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:112" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:112" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>27</v>
       </c>
@@ -3404,7 +3403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:112" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:112" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>29</v>
       </c>
@@ -3425,9 +3424,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:112" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:112" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>6</v>
@@ -3446,12 +3445,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:112" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:112" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="C23" s="29">
         <v>45404</v>
@@ -3467,9 +3466,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:112" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:112" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>28</v>
@@ -3488,19 +3487,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:112" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:112" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C25" s="29">
-        <v>45417</v>
+        <f>D24+1</f>
+        <v>45418</v>
       </c>
       <c r="D25" s="30">
         <f t="shared" si="6"/>
-        <v>45417</v>
+        <v>45418</v>
       </c>
       <c r="E25" s="7">
         <v>1</v>
@@ -3509,9 +3509,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:112" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:112" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>6</v>
@@ -3530,18 +3530,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:112" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:112" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C27" s="29">
         <v>45418</v>
       </c>
       <c r="D27" s="30">
-        <f t="shared" ref="D27:D33" si="7">C27+E27-1</f>
+        <f t="shared" ref="D27:D32" si="7">C27+E27-1</f>
         <v>45431</v>
       </c>
       <c r="E27" s="7">
@@ -3551,9 +3551,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:112" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:112" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>28</v>
@@ -3572,7 +3572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:112" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:112" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>27</v>
       </c>
@@ -3593,19 +3593,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:112" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:112" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C30" s="29">
-        <v>45424</v>
+        <f>D28+1</f>
+        <v>45432</v>
       </c>
       <c r="D30" s="30">
         <f t="shared" si="7"/>
-        <v>45424</v>
+        <v>45432</v>
       </c>
       <c r="E30" s="7">
         <v>1</v>
@@ -3614,9 +3615,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:112" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:112" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>15</v>
@@ -3635,9 +3636,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:112" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:112" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>15</v>
@@ -3656,7 +3657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="16" customFormat="1" ht="10.199999999999999" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" s="16" customFormat="1" ht="10.15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="29"/>
@@ -3666,7 +3667,7 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
-  <autoFilter ref="A3:IK33" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A3:IK33">
     <filterColumn colId="7" showButton="0"/>
     <filterColumn colId="8" showButton="0"/>
     <filterColumn colId="9" showButton="0"/>
@@ -3873,12 +3874,18 @@
     <filterColumn colId="243" showButton="0"/>
   </autoFilter>
   <mergeCells count="34">
-    <mergeCell ref="AJ3:AP3"/>
-    <mergeCell ref="AQ3:AW3"/>
-    <mergeCell ref="H3:N3"/>
-    <mergeCell ref="O3:U3"/>
-    <mergeCell ref="V3:AB3"/>
-    <mergeCell ref="AC3:AI3"/>
+    <mergeCell ref="HX3:ID3"/>
+    <mergeCell ref="AX3:BD3"/>
+    <mergeCell ref="CN3:CT3"/>
+    <mergeCell ref="CU3:DA3"/>
+    <mergeCell ref="DB3:DH3"/>
+    <mergeCell ref="ED3:EJ3"/>
+    <mergeCell ref="BE3:BK3"/>
+    <mergeCell ref="HQ3:HW3"/>
+    <mergeCell ref="GO3:GU3"/>
+    <mergeCell ref="GV3:HB3"/>
+    <mergeCell ref="FT3:FZ3"/>
+    <mergeCell ref="GA3:GG3"/>
     <mergeCell ref="IE3:IK3"/>
     <mergeCell ref="BL3:BR3"/>
     <mergeCell ref="BS3:BY3"/>
@@ -3895,18 +3902,12 @@
     <mergeCell ref="GH3:GN3"/>
     <mergeCell ref="FF3:FL3"/>
     <mergeCell ref="FM3:FS3"/>
-    <mergeCell ref="HX3:ID3"/>
-    <mergeCell ref="AX3:BD3"/>
-    <mergeCell ref="CN3:CT3"/>
-    <mergeCell ref="CU3:DA3"/>
-    <mergeCell ref="DB3:DH3"/>
-    <mergeCell ref="ED3:EJ3"/>
-    <mergeCell ref="BE3:BK3"/>
-    <mergeCell ref="HQ3:HW3"/>
-    <mergeCell ref="GO3:GU3"/>
-    <mergeCell ref="GV3:HB3"/>
-    <mergeCell ref="FT3:FZ3"/>
-    <mergeCell ref="GA3:GG3"/>
+    <mergeCell ref="AJ3:AP3"/>
+    <mergeCell ref="AQ3:AW3"/>
+    <mergeCell ref="H3:N3"/>
+    <mergeCell ref="O3:U3"/>
+    <mergeCell ref="V3:AB3"/>
+    <mergeCell ref="AC3:AI3"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="H4:IK4">
@@ -3947,13 +3948,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:colOff>47625</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>23813</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>381000</xdr:colOff>
+                    <xdr:colOff>138113</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </to>
@@ -3969,7 +3970,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Blad3"/>
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -3977,14 +3978,14 @@
       <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
         <v>4</v>
       </c>

</xml_diff>